<commit_message>
update WATCHLIST for price, trend, and rsi vals
</commit_message>
<xml_diff>
--- a/__testing/portfolio.xlsx
+++ b/__testing/portfolio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\OneDrive\PET PROJECTS\Al-the-Trader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_CAE6C32C0F51D32650D099EDB054F94F936453A4" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{BE8C11A1-5BE3-46F6-9E77-A3B620C91899}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_9AEA69BC0CEE76852F6AD0F83F14E9F7C3EC2658" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{F68859F4-64FC-4E38-8A9C-DBD0A73EE7BD}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="2784" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="watchlist" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
   <si>
     <t>ticker</t>
   </si>
@@ -146,6 +146,9 @@
     <t>STOCKS</t>
   </si>
   <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
     <t>date</t>
   </si>
   <si>
@@ -165,6 +168,54 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>01/05/2020 18:02:19</t>
+  </si>
+  <si>
+    <t>02/05/2020 06:30:28</t>
+  </si>
+  <si>
+    <t>02/05/2020 06:35:22</t>
+  </si>
+  <si>
+    <t>02/05/2020 07:35:22</t>
+  </si>
+  <si>
+    <t>04/05/2020 09:35:32</t>
+  </si>
+  <si>
+    <t>04/05/2020 10:35:22</t>
+  </si>
+  <si>
+    <t>04/05/2020 11:35:23</t>
+  </si>
+  <si>
+    <t>04/05/2020 12:57:22</t>
+  </si>
+  <si>
+    <t>04/05/2020 13:06:21</t>
+  </si>
+  <si>
+    <t>04/05/2020 13:35:27</t>
+  </si>
+  <si>
+    <t>04/05/2020 14:35:26</t>
+  </si>
+  <si>
+    <t>04/05/2020 15:35:19</t>
+  </si>
+  <si>
+    <t>04/05/2020 16:07:30</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>pct_change</t>
+  </si>
+  <si>
+    <t>rsi</t>
   </si>
 </sst>
 </file>
@@ -527,256 +578,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
@@ -818,16 +788,16 @@
         <v>24</v>
       </c>
       <c r="B2">
-        <v>96.05</v>
+        <v>96.87</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
       <c r="D2">
-        <v>960.5</v>
+        <v>968.7</v>
       </c>
       <c r="E2">
-        <v>24.711111111111119</v>
+        <v>22.5840707964602</v>
       </c>
       <c r="F2" t="s">
         <v>36</v>
@@ -838,16 +808,16 @@
         <v>28</v>
       </c>
       <c r="B3">
-        <v>41.66</v>
+        <v>42.65</v>
       </c>
       <c r="C3">
         <v>24</v>
       </c>
       <c r="D3">
-        <v>999.83999999999992</v>
+        <v>1023.6</v>
       </c>
       <c r="E3">
-        <v>28.551107498475911</v>
+        <v>27.762557077625569</v>
       </c>
       <c r="F3" t="s">
         <v>36</v>
@@ -860,7 +830,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -887,7 +857,15 @@
         <v>39</v>
       </c>
       <c r="B3">
-        <v>1960.34</v>
+        <v>1992.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>10031.959999999999</v>
       </c>
     </row>
   </sheetData>
@@ -905,13 +883,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>32</v>
@@ -925,7 +903,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>24</v>
@@ -945,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
         <v>28</v>
@@ -966,30 +944,210 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543C7E2F-024B-49CE-9D69-1560F225A8CD}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>8039.66</v>
+      </c>
+      <c r="C2">
+        <v>1960.34</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3">
+        <v>8039.66</v>
+      </c>
+      <c r="C3">
+        <v>1960.34</v>
+      </c>
+      <c r="D3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>8039.66</v>
+      </c>
+      <c r="C4">
+        <v>1960.34</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5">
+        <v>8039.66</v>
+      </c>
+      <c r="C5">
+        <v>1960.34</v>
+      </c>
+      <c r="D5">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>8039.66</v>
+      </c>
+      <c r="C6">
+        <v>1927.38</v>
+      </c>
+      <c r="D6">
+        <v>9967.0400000000009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7">
+        <v>8039.66</v>
+      </c>
+      <c r="C7">
+        <v>1951.96</v>
+      </c>
+      <c r="D7">
+        <v>9991.619999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8">
+        <v>8039.66</v>
+      </c>
+      <c r="C8">
+        <v>1972.36</v>
+      </c>
+      <c r="D8">
+        <v>10012.02</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9">
+        <v>8039.66</v>
+      </c>
+      <c r="C9">
+        <v>1970.36</v>
+      </c>
+      <c r="D9">
+        <v>10010.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10">
+        <v>8039.66</v>
+      </c>
+      <c r="C10">
+        <v>1968.6</v>
+      </c>
+      <c r="D10">
+        <v>10008.26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11">
+        <v>8039.66</v>
+      </c>
+      <c r="C11">
+        <v>1975.52</v>
+      </c>
+      <c r="D11">
+        <v>10015.18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12">
+        <v>8039.66</v>
+      </c>
+      <c r="C12">
+        <v>1974.18</v>
+      </c>
+      <c r="D12">
+        <v>10013.84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13">
+        <v>8039.66</v>
+      </c>
+      <c r="C13">
+        <v>1992.3</v>
+      </c>
+      <c r="D13">
+        <v>10031.959999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>8039.66</v>
+      </c>
+      <c r="C14">
+        <v>1992.3</v>
+      </c>
+      <c r="D14">
+        <v>10031.959999999999</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finalize google sheet migration
</commit_message>
<xml_diff>
--- a/__testing/portfolio.xlsx
+++ b/__testing/portfolio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\OneDrive\PET PROJECTS\Al-the-Trader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9cefadc21042b88c/PET_PROJECTS/Al-the-Trader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_B0A5AAA6EA16F6A9E5FADCB10392DD110A25B745" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{90733D49-C59D-4BB2-AFA7-D01FCA06BDE1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{D393F9D2-285A-41ED-9F07-FD42D3DAFCF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="2784" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="watchlist" sheetId="1" r:id="rId1"/>
@@ -19,20 +19,12 @@
     <sheet name="trades" sheetId="4" r:id="rId4"/>
     <sheet name="summary" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="141">
   <si>
     <t>ticker</t>
   </si>
@@ -46,94 +38,97 @@
     <t>rsi</t>
   </si>
   <si>
+    <t>XOM</t>
+  </si>
+  <si>
+    <t>CVX</t>
+  </si>
+  <si>
+    <t>AXP</t>
+  </si>
+  <si>
+    <t>WBA</t>
+  </si>
+  <si>
+    <t>NKE</t>
+  </si>
+  <si>
+    <t>UNH</t>
+  </si>
+  <si>
+    <t>MMM</t>
+  </si>
+  <si>
+    <t>RTX</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>IBM</t>
+  </si>
+  <si>
     <t>TRV</t>
   </si>
   <si>
+    <t>JPM</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>MRK</t>
+  </si>
+  <si>
+    <t>KO</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>DOW</t>
+  </si>
+  <si>
+    <t>MCD</t>
+  </si>
+  <si>
+    <t>INTC</t>
+  </si>
+  <si>
+    <t>VZ</t>
+  </si>
+  <si>
     <t>CAT</t>
   </si>
   <si>
-    <t>WBA</t>
+    <t>HD</t>
+  </si>
+  <si>
+    <t>JNJ</t>
   </si>
   <si>
     <t>CSCO</t>
   </si>
   <si>
-    <t>RTX</t>
-  </si>
-  <si>
-    <t>IBM</t>
+    <t>PFE</t>
+  </si>
+  <si>
+    <t>AAPL</t>
+  </si>
+  <si>
+    <t>MSFT</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>DIS</t>
   </si>
   <si>
     <t>WMT</t>
   </si>
   <si>
-    <t>MRK</t>
-  </si>
-  <si>
-    <t>JPM</t>
-  </si>
-  <si>
-    <t>DIS</t>
-  </si>
-  <si>
-    <t>BA</t>
-  </si>
-  <si>
-    <t>XOM</t>
-  </si>
-  <si>
-    <t>UNH</t>
-  </si>
-  <si>
-    <t>KO</t>
-  </si>
-  <si>
-    <t>DOW</t>
-  </si>
-  <si>
-    <t>CVX</t>
-  </si>
-  <si>
-    <t>GS</t>
-  </si>
-  <si>
-    <t>VZ</t>
-  </si>
-  <si>
-    <t>INTC</t>
-  </si>
-  <si>
-    <t>MSFT</t>
-  </si>
-  <si>
-    <t>PFE</t>
-  </si>
-  <si>
-    <t>AXP</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>MCD</t>
-  </si>
-  <si>
-    <t>MMM</t>
-  </si>
-  <si>
-    <t>NKE</t>
-  </si>
-  <si>
-    <t>PG</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>JNJ</t>
-  </si>
-  <si>
-    <t>HD</t>
+    <t>purch_price</t>
   </si>
   <si>
     <t>current_price</t>
@@ -145,6 +140,9 @@
     <t>value</t>
   </si>
   <si>
+    <t>performance</t>
+  </si>
+  <si>
     <t>current_rsi</t>
   </si>
   <si>
@@ -181,6 +179,147 @@
     <t>05/05/2020 09:35:14</t>
   </si>
   <si>
+    <t>05/05/2020 15:35:05</t>
+  </si>
+  <si>
+    <t>06/05/2020 09:35:11</t>
+  </si>
+  <si>
+    <t>06/05/2020 11:35:12</t>
+  </si>
+  <si>
+    <t>06/05/2020 12:35:05</t>
+  </si>
+  <si>
+    <t>12/05/2020 07:49:21</t>
+  </si>
+  <si>
+    <t>12/05/2020 07:49:24</t>
+  </si>
+  <si>
+    <t>12/05/2020 09:35:10</t>
+  </si>
+  <si>
+    <t>12/05/2020 14:35:11</t>
+  </si>
+  <si>
+    <t>12/05/2020 17:35:15</t>
+  </si>
+  <si>
+    <t>13/05/2020 09:35:40</t>
+  </si>
+  <si>
+    <t>13/05/2020 10:35:18</t>
+  </si>
+  <si>
+    <t>13/05/2020 10:35:20</t>
+  </si>
+  <si>
+    <t>13/05/2020 10:35:28</t>
+  </si>
+  <si>
+    <t>13/05/2020 13:03:20</t>
+  </si>
+  <si>
+    <t>13/05/2020 13:03:21</t>
+  </si>
+  <si>
+    <t>13/05/2020 13:35:25</t>
+  </si>
+  <si>
+    <t>14/05/2020 09:35:49</t>
+  </si>
+  <si>
+    <t>sell</t>
+  </si>
+  <si>
+    <t>26/05/2020 12:28:56</t>
+  </si>
+  <si>
+    <t>26/05/2020 12:29:00</t>
+  </si>
+  <si>
+    <t>27/05/2020 11:02:26</t>
+  </si>
+  <si>
+    <t>27/05/2020 11:02:28</t>
+  </si>
+  <si>
+    <t>27/05/2020 11:02:31</t>
+  </si>
+  <si>
+    <t>27/05/2020 11:02:32</t>
+  </si>
+  <si>
+    <t>27/05/2020 11:02:33</t>
+  </si>
+  <si>
+    <t>27/05/2020 11:02:34</t>
+  </si>
+  <si>
+    <t>27/05/2020 11:02:37</t>
+  </si>
+  <si>
+    <t>27/05/2020 11:02:38</t>
+  </si>
+  <si>
+    <t>28/05/2020 09:53:16</t>
+  </si>
+  <si>
+    <t>28/05/2020 10:04:14</t>
+  </si>
+  <si>
+    <t>28/05/2020 10:04:16</t>
+  </si>
+  <si>
+    <t>28/05/2020 10:04:17</t>
+  </si>
+  <si>
+    <t>28/05/2020 10:04:23</t>
+  </si>
+  <si>
+    <t>28/05/2020 10:04:25</t>
+  </si>
+  <si>
+    <t>01/06/2020 18:33:01</t>
+  </si>
+  <si>
+    <t>02/06/2020 18:50:13</t>
+  </si>
+  <si>
+    <t>03/06/2020 18:22:42</t>
+  </si>
+  <si>
+    <t>05/06/2020 12:11:52</t>
+  </si>
+  <si>
+    <t>12/06/2020 13:59:22</t>
+  </si>
+  <si>
+    <t>12/06/2020 13:59:23</t>
+  </si>
+  <si>
+    <t>12/06/2020 13:59:31</t>
+  </si>
+  <si>
+    <t>19/06/2020 20:02:07</t>
+  </si>
+  <si>
+    <t>19/06/2020 20:02:12</t>
+  </si>
+  <si>
+    <t>29/06/2020 17:43:44</t>
+  </si>
+  <si>
+    <t>29/06/2020 17:43:49</t>
+  </si>
+  <si>
+    <t>09/07/2020 17:28:44</t>
+  </si>
+  <si>
+    <t>09/07/2020 17:28:45</t>
+  </si>
+  <si>
     <t>cash</t>
   </si>
   <si>
@@ -199,26 +338,122 @@
     <t>04/05/2020 17:38:22</t>
   </si>
   <si>
-    <t>05/05/2020 09:35:16</t>
-  </si>
-  <si>
-    <t>05/05/2020 10:35:09</t>
-  </si>
-  <si>
-    <t>05/05/2020 14:02:43</t>
-  </si>
-  <si>
-    <t>purch_price</t>
-  </si>
-  <si>
-    <t>performance</t>
+    <t>05/05/2020 16:35:30</t>
+  </si>
+  <si>
+    <t>06/05/2020 17:35:03</t>
+  </si>
+  <si>
+    <t>07/05/2020 18:35:02</t>
+  </si>
+  <si>
+    <t>08/05/2020 16:35:02</t>
+  </si>
+  <si>
+    <t>09/05/2020 06:02:00</t>
+  </si>
+  <si>
+    <t>11/05/2020 17:35:02</t>
+  </si>
+  <si>
+    <t>12/05/2020 19:35:03</t>
+  </si>
+  <si>
+    <t>13/05/2020 18:35:07</t>
+  </si>
+  <si>
+    <t>14/05/2020 15:35:07</t>
+  </si>
+  <si>
+    <t>15/05/2020 05:44:59</t>
+  </si>
+  <si>
+    <t>25/05/2020 09:35:10</t>
+  </si>
+  <si>
+    <t>26/05/2020 17:35:11</t>
+  </si>
+  <si>
+    <t>27/05/2020 18:44:05</t>
+  </si>
+  <si>
+    <t>28/05/2020 17:04:00</t>
+  </si>
+  <si>
+    <t>29/05/2020 18:32:43</t>
+  </si>
+  <si>
+    <t>01/06/2020 18:32:57</t>
+  </si>
+  <si>
+    <t>02/06/2020 18:50:11</t>
+  </si>
+  <si>
+    <t>03/06/2020 18:22:41</t>
+  </si>
+  <si>
+    <t>05/06/2020 16:57:59</t>
+  </si>
+  <si>
+    <t>08/06/2020 16:37:45</t>
+  </si>
+  <si>
+    <t>09/06/2020 18:08:41</t>
+  </si>
+  <si>
+    <t>10/06/2020 17:20:06</t>
+  </si>
+  <si>
+    <t>12/06/2020 13:59:17</t>
+  </si>
+  <si>
+    <t>14/06/2020 06:29:50</t>
+  </si>
+  <si>
+    <t>15/06/2020 17:49:50</t>
+  </si>
+  <si>
+    <t>16/06/2020 13:02:42</t>
+  </si>
+  <si>
+    <t>19/06/2020 20:01:48</t>
+  </si>
+  <si>
+    <t>29/06/2020 17:43:25</t>
+  </si>
+  <si>
+    <t>30/06/2020 16:55:00</t>
+  </si>
+  <si>
+    <t>01/07/2020 18:35:15</t>
+  </si>
+  <si>
+    <t>02/07/2020 17:51:31</t>
+  </si>
+  <si>
+    <t>03/07/2020 17:55:02</t>
+  </si>
+  <si>
+    <t>06/07/2020 16:57:17</t>
+  </si>
+  <si>
+    <t>07/07/2020 17:15:38</t>
+  </si>
+  <si>
+    <t>08/07/2020 20:00:23</t>
+  </si>
+  <si>
+    <t>09/07/2020 17:28:26</t>
+  </si>
+  <si>
+    <t>10/07/2020 16:50:27</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,12 +465,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -273,12 +502,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -585,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,13 +836,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>98.09</v>
+        <v>42.65</v>
       </c>
       <c r="C2">
-        <v>1.2176</v>
+        <v>3.1190000000000002</v>
       </c>
       <c r="D2">
-        <v>22.39025827359325</v>
+        <v>35.450346420323307</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -624,13 +850,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>110.35</v>
+        <v>85.23</v>
       </c>
       <c r="C3">
-        <v>2.4415</v>
+        <v>3.0093999999999999</v>
       </c>
       <c r="D3">
-        <v>30.036844259898249</v>
+        <v>37.924757281553418</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -638,13 +864,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>42.12</v>
+        <v>93.23</v>
       </c>
       <c r="C4">
-        <v>-0.77739999999999998</v>
+        <v>2.9369999999999998</v>
       </c>
       <c r="D4">
-        <v>32.20755983001564</v>
+        <v>38.453038674033181</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -652,13 +878,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>41.35</v>
+        <v>40.119999999999997</v>
       </c>
       <c r="C5">
-        <v>1.0508</v>
+        <v>2.8454000000000002</v>
       </c>
       <c r="D5">
-        <v>39.372409709887542</v>
+        <v>41.489361702127638</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,13 +892,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>58.85</v>
+        <v>97.99</v>
       </c>
       <c r="C6">
-        <v>-3.6981999999999999</v>
+        <v>1.0309999999999999</v>
       </c>
       <c r="D6">
-        <v>39.47023341201151</v>
+        <v>42.52520824199911</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,13 +906,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>121.68</v>
+        <v>291.23</v>
       </c>
       <c r="C7">
-        <v>-0.15590000000000001</v>
+        <v>2.4E-2</v>
       </c>
       <c r="D7">
-        <v>39.578947368421069</v>
+        <v>43.825785696609763</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,13 +920,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>123.7</v>
+        <v>152.85</v>
       </c>
       <c r="C8">
-        <v>0.63460000000000005</v>
+        <v>0.9244</v>
       </c>
       <c r="D8">
-        <v>40.718562874251489</v>
+        <v>44.615384615384627</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -708,13 +934,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>78.14</v>
+        <v>59.64</v>
       </c>
       <c r="C9">
-        <v>1.6654</v>
+        <v>2.6328999999999998</v>
       </c>
       <c r="D9">
-        <v>40.812182741116757</v>
+        <v>44.756277695716392</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -722,13 +948,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>93.51</v>
+        <v>192.55</v>
       </c>
       <c r="C10">
-        <v>1.4869000000000001</v>
+        <v>0.1769</v>
       </c>
       <c r="D10">
-        <v>40.974039042060809</v>
+        <v>46.567450792126778</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -736,13 +962,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>104.58</v>
+        <v>118.35</v>
       </c>
       <c r="C11">
-        <v>1.3569</v>
+        <v>2.2816000000000001</v>
       </c>
       <c r="D11">
-        <v>40.97835430178948</v>
+        <v>47.961630695443617</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -750,13 +976,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>131.46</v>
+        <v>113.84</v>
       </c>
       <c r="C12">
-        <v>-1.4320999999999999</v>
+        <v>3.4533</v>
       </c>
       <c r="D12">
-        <v>41.256777314038317</v>
+        <v>48.059701492537307</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,13 +990,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>44.88</v>
+        <v>96.27</v>
       </c>
       <c r="C13">
-        <v>4.0334000000000003</v>
+        <v>5.4667000000000003</v>
       </c>
       <c r="D13">
-        <v>41.71095925082259</v>
+        <v>48.226270373921359</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -778,13 +1004,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>287.54000000000002</v>
+        <v>205.56</v>
       </c>
       <c r="C14">
-        <v>1.0649999999999999</v>
+        <v>4.4352999999999998</v>
       </c>
       <c r="D14">
-        <v>42.897938912341708</v>
+        <v>48.749187784275513</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -792,13 +1018,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>45.14</v>
+        <v>76.73</v>
       </c>
       <c r="C15">
-        <v>-1.0087999999999999</v>
+        <v>5.2200000000000003E-2</v>
       </c>
       <c r="D15">
-        <v>44.061100869107143</v>
+        <v>50.919540229885122</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -806,13 +1032,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>33.06</v>
+        <v>45.15</v>
       </c>
       <c r="C16">
-        <v>-2.5640999999999998</v>
+        <v>2.8239999999999998</v>
       </c>
       <c r="D16">
-        <v>44.139316811788348</v>
+        <v>51.971326164874547</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -820,13 +1046,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>91.44</v>
+        <v>178.44</v>
       </c>
       <c r="C17">
-        <v>2.2361</v>
+        <v>2.9777999999999998</v>
       </c>
       <c r="D17">
-        <v>44.421380384016587</v>
+        <v>52.428376534788541</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -834,13 +1060,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>176.03</v>
+        <v>40.76</v>
       </c>
       <c r="C18">
-        <v>-0.60419999999999996</v>
+        <v>3.3469000000000002</v>
       </c>
       <c r="D18">
-        <v>45.541048904624901</v>
+        <v>55.118110236220481</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -848,13 +1074,13 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>56.24</v>
+        <v>184.88</v>
       </c>
       <c r="C19">
-        <v>-1.0382</v>
+        <v>0.2984</v>
       </c>
       <c r="D19">
-        <v>45.871024219433927</v>
+        <v>55.626326963906621</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -862,13 +1088,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>57.99</v>
+        <v>59.53</v>
       </c>
       <c r="C20">
-        <v>0.90480000000000005</v>
+        <v>1.9</v>
       </c>
       <c r="D20">
-        <v>47.881224868543157</v>
+        <v>56.439393939393973</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -876,13 +1102,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>178.84</v>
+        <v>54.49</v>
       </c>
       <c r="C21">
-        <v>2.4460000000000002</v>
+        <v>1.0197000000000001</v>
       </c>
       <c r="D21">
-        <v>51.715243745163768</v>
+        <v>56.761268781302178</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -890,13 +1116,13 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>37.619999999999997</v>
+        <v>128.01</v>
       </c>
       <c r="C22">
-        <v>-5.3100000000000001E-2</v>
+        <v>1.8133999999999999</v>
       </c>
       <c r="D22">
-        <v>51.803278688524593</v>
+        <v>59.126106194690273</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -904,13 +1130,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>86.38</v>
+        <v>250.11</v>
       </c>
       <c r="C23">
-        <v>-2.1966000000000001</v>
+        <v>0.86709999999999998</v>
       </c>
       <c r="D23">
-        <v>52.891370924157812</v>
+        <v>59.456217512994847</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -918,13 +1144,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>293.16000000000003</v>
+        <v>142.37</v>
       </c>
       <c r="C24">
-        <v>1.4149</v>
+        <v>-8.4199999999999997E-2</v>
       </c>
       <c r="D24">
-        <v>54.15306939227878</v>
+        <v>65.033407572383197</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -932,13 +1158,13 @@
         <v>27</v>
       </c>
       <c r="B25">
-        <v>181.87</v>
+        <v>46.66</v>
       </c>
       <c r="C25">
-        <v>-0.4325</v>
+        <v>-8.5699999999999998E-2</v>
       </c>
       <c r="D25">
-        <v>55.083868295713401</v>
+        <v>67.652859960552206</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -946,13 +1172,13 @@
         <v>28</v>
       </c>
       <c r="B26">
-        <v>148.4</v>
+        <v>33.83</v>
       </c>
       <c r="C26">
-        <v>-0.1346</v>
+        <v>1.1057999999999999</v>
       </c>
       <c r="D26">
-        <v>57.731213872832363</v>
+        <v>68.105515587529965</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -960,13 +1186,13 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>85.75</v>
+        <v>383.68</v>
       </c>
       <c r="C27">
-        <v>0.2455</v>
+        <v>0.1749</v>
       </c>
       <c r="D27">
-        <v>58.684128468974102</v>
+        <v>70.951957295373688</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -974,13 +1200,13 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>115.77</v>
+        <v>213.67</v>
       </c>
       <c r="C28">
-        <v>-0.89880000000000004</v>
+        <v>-0.30330000000000001</v>
       </c>
       <c r="D28">
-        <v>59.798994974874347</v>
+        <v>74.192377495462807</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -988,13 +1214,13 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>176.15</v>
+        <v>123.89</v>
       </c>
       <c r="C29">
-        <v>0.33040000000000003</v>
+        <v>1.1512</v>
       </c>
       <c r="D29">
-        <v>62.925944865417719</v>
+        <v>74.71169686985175</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1002,13 +1228,13 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>148.27000000000001</v>
+        <v>119.34</v>
       </c>
       <c r="C30">
-        <v>-1.35E-2</v>
+        <v>2.1659000000000002</v>
       </c>
       <c r="D30">
-        <v>70.267368194996351</v>
+        <v>75.285171102661593</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1016,13 +1242,13 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>221.84</v>
+        <v>130.68</v>
       </c>
       <c r="C31">
-        <v>1.4961</v>
+        <v>2.2934999999999999</v>
       </c>
       <c r="D31">
-        <v>73.793329509137095</v>
+        <v>76.690997566909971</v>
       </c>
     </row>
   </sheetData>
@@ -1032,124 +1258,248 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>58</v>
+      <c r="B1" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>59</v>
+        <v>37</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>96.05</v>
+        <v>149.11000000000001</v>
       </c>
       <c r="C2">
-        <v>98.09</v>
+        <v>142.37</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E2">
-        <v>980.90000000000009</v>
+        <v>427.11</v>
       </c>
       <c r="F2">
-        <v>2.1238938053097511E-2</v>
+        <v>-4.5202</v>
       </c>
       <c r="G2">
-        <v>22.39025827359325</v>
+        <v>65.033407572383197</v>
       </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="B3">
-        <v>41.66</v>
+        <v>35.46</v>
       </c>
       <c r="C3">
-        <v>42.12</v>
+        <v>33.83</v>
       </c>
       <c r="D3">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3">
-        <v>1010.88</v>
+        <v>778.08999999999992</v>
       </c>
       <c r="F3">
-        <v>1.1041766682669207E-2</v>
+        <v>-4.5967000000000002</v>
       </c>
       <c r="G3">
-        <v>32.20755983001564</v>
+        <v>68.105515587529965</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>58.26</v>
+      </c>
+      <c r="C4">
+        <v>59.53</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>833.42000000000007</v>
+      </c>
+      <c r="F4">
+        <v>2.1798999999999999</v>
+      </c>
+      <c r="G4">
+        <v>56.439393939393973</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>278.89</v>
+      </c>
+      <c r="C5">
+        <v>291.23</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>873.69</v>
+      </c>
+      <c r="F5">
+        <v>4.4246999999999996</v>
+      </c>
+      <c r="G5">
+        <v>43.825785696609763</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>45.98</v>
+      </c>
+      <c r="C6">
+        <v>42.65</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>511.8</v>
+      </c>
+      <c r="F6">
+        <v>-7.2423000000000002</v>
+      </c>
+      <c r="G6">
+        <v>35.450346420323307</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>97.81</v>
+      </c>
+      <c r="C7">
+        <v>96.27</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>577.62</v>
+      </c>
+      <c r="F7">
+        <v>-1.5745</v>
+      </c>
+      <c r="G7">
+        <v>48.226270373921359</v>
+      </c>
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>61.92</v>
+      </c>
+      <c r="C8">
+        <v>59.64</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>417.48</v>
+      </c>
+      <c r="F8">
+        <v>-3.6821999999999999</v>
+      </c>
+      <c r="G8">
+        <v>44.756277695716392</v>
+      </c>
+      <c r="H8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>94.52</v>
+      </c>
+      <c r="C9">
+        <v>93.23</v>
+      </c>
+      <c r="D9">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>110.2</v>
-      </c>
-      <c r="C4">
-        <v>110.35</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>772.44999999999993</v>
-      </c>
-      <c r="F4">
-        <v>1.3611615245008313E-3</v>
-      </c>
-      <c r="G4">
-        <v>30.036844259898249</v>
-      </c>
-      <c r="H4" t="s">
-        <v>39</v>
+      <c r="E9">
+        <v>466.15</v>
+      </c>
+      <c r="F9">
+        <v>-1.3648</v>
+      </c>
+      <c r="G9">
+        <v>38.453038674033181</v>
+      </c>
+      <c r="H9" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1163,34 +1513,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B2">
-        <v>7268.26</v>
+        <v>5740.5700000000024</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B3">
-        <v>2764.23</v>
+        <v>4885.3600000000006</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B4">
-        <v>10032.49</v>
+        <v>10625.93</v>
       </c>
     </row>
   </sheetData>
@@ -1200,43 +1550,41 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G4"/>
-    </sheetView>
+    <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E2">
         <v>10</v>
@@ -1244,23 +1592,19 @@
       <c r="F2">
         <v>960.5</v>
       </c>
-      <c r="G2">
-        <f>F2/E2</f>
-        <v>96.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E3">
         <v>24</v>
@@ -1268,23 +1612,19 @@
       <c r="F3">
         <v>999.83999999999992</v>
       </c>
-      <c r="G3">
-        <f>F3/E3</f>
-        <v>41.66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E4">
         <v>7</v>
@@ -1292,9 +1632,945 @@
       <c r="F4">
         <v>771.4</v>
       </c>
-      <c r="G4">
-        <f>F4/E4</f>
-        <v>110.2</v>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>708.59999999999991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6">
+        <v>11</v>
+      </c>
+      <c r="F6">
+        <v>622.04999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>499.28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>458.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <v>467.46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>447.33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>352.76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>176.54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>297.81000000000012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>237.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>265.86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>241.98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>172.09</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>120.81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20">
+        <v>172.29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>124.34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="F22">
+        <v>129.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>152.52000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>187.24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25">
+        <v>398.96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>310.83999999999997</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>203.71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+      <c r="F28">
+        <v>294.06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>847.35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>144.54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31">
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>1063.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>68</v>
+      </c>
+      <c r="E32">
+        <v>24</v>
+      </c>
+      <c r="F32">
+        <v>1021.68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>673.19999999999993</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" t="s">
+        <v>68</v>
+      </c>
+      <c r="E34">
+        <v>5</v>
+      </c>
+      <c r="F34">
+        <v>195.05</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>251.18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="F36">
+        <v>189.09</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37">
+        <v>6</v>
+      </c>
+      <c r="F37">
+        <v>281.76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38">
+        <v>23</v>
+      </c>
+      <c r="F38">
+        <v>815.58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39">
+        <v>5</v>
+      </c>
+      <c r="F39">
+        <v>619.70000000000005</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>31</v>
+      </c>
+      <c r="D40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40">
+        <v>4</v>
+      </c>
+      <c r="F40">
+        <v>474.12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41">
+        <v>6</v>
+      </c>
+      <c r="F41">
+        <v>492.36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42">
+        <v>11</v>
+      </c>
+      <c r="F42">
+        <v>636.46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" t="s">
+        <v>41</v>
+      </c>
+      <c r="E43">
+        <v>14</v>
+      </c>
+      <c r="F43">
+        <v>815.64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
+        <v>41</v>
+      </c>
+      <c r="E44">
+        <v>3</v>
+      </c>
+      <c r="F44">
+        <v>836.67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45">
+        <v>18</v>
+      </c>
+      <c r="F45">
+        <v>795.24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46">
+        <v>12</v>
+      </c>
+      <c r="F46">
+        <v>551.76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>93</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47">
+        <v>6</v>
+      </c>
+      <c r="F47">
+        <v>586.86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <v>433.44</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49">
+        <v>5</v>
+      </c>
+      <c r="F49">
+        <v>472.6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>96</v>
+      </c>
+      <c r="C50" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" t="s">
+        <v>68</v>
+      </c>
+      <c r="E50">
+        <v>18</v>
+      </c>
+      <c r="F50">
+        <v>840.6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" t="s">
+        <v>33</v>
+      </c>
+      <c r="D51" t="s">
+        <v>68</v>
+      </c>
+      <c r="E51">
+        <v>8</v>
+      </c>
+      <c r="F51">
+        <v>1022</v>
       </c>
     </row>
   </sheetData>
@@ -1304,29 +2580,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>51</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="B2">
         <v>8039.66</v>
@@ -1340,7 +2618,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>102</v>
       </c>
       <c r="B3">
         <v>8039.66</v>
@@ -1354,7 +2632,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="B4">
         <v>8039.66</v>
@@ -1368,44 +2646,520 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="B5">
-        <v>7268.26</v>
+        <v>6559.66</v>
       </c>
       <c r="C5">
-        <v>2776.38</v>
+        <v>3447.35</v>
       </c>
       <c r="D5">
-        <v>10044.64</v>
+        <v>10007.01</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="B6">
-        <v>7268.26</v>
+        <v>4979.93</v>
       </c>
       <c r="C6">
-        <v>2764.23</v>
+        <v>4928.07</v>
       </c>
       <c r="D6">
-        <v>10032.49</v>
+        <v>9908</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="B7">
-        <v>7268.26</v>
+        <v>4979.93</v>
       </c>
       <c r="C7">
-        <v>2764.23</v>
+        <v>4916.6100000000006</v>
       </c>
       <c r="D7">
-        <v>10032.49</v>
+        <v>9896.5400000000009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8">
+        <v>4979.93</v>
+      </c>
+      <c r="C8">
+        <v>5044.8500000000004</v>
+      </c>
+      <c r="D8">
+        <v>10024.780000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9">
+        <v>4979.93</v>
+      </c>
+      <c r="C9">
+        <v>5044.8500000000004</v>
+      </c>
+      <c r="D9">
+        <v>10024.780000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10">
+        <v>4979.93</v>
+      </c>
+      <c r="C10">
+        <v>4981.0499999999993</v>
+      </c>
+      <c r="D10">
+        <v>9960.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11">
+        <v>3242.84</v>
+      </c>
+      <c r="C11">
+        <v>6603.5999999999995</v>
+      </c>
+      <c r="D11">
+        <v>9846.4399999999987</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12">
+        <v>1734.2</v>
+      </c>
+      <c r="C12">
+        <v>7930.2000000000007</v>
+      </c>
+      <c r="D12">
+        <v>9664.4000000000015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13">
+        <v>1858.54</v>
+      </c>
+      <c r="C13">
+        <v>7851.4400000000014</v>
+      </c>
+      <c r="D13">
+        <v>9709.98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14">
+        <v>1858.54</v>
+      </c>
+      <c r="C14">
+        <v>7897.78</v>
+      </c>
+      <c r="D14">
+        <v>9756.32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15">
+        <v>1858.54</v>
+      </c>
+      <c r="C15">
+        <v>8207.9500000000007</v>
+      </c>
+      <c r="D15">
+        <v>10066.49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16">
+        <v>2140.56</v>
+      </c>
+      <c r="C16">
+        <v>8223.31</v>
+      </c>
+      <c r="D16">
+        <v>10363.870000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17">
+        <v>5590.56</v>
+      </c>
+      <c r="C17">
+        <v>4948.5300000000007</v>
+      </c>
+      <c r="D17">
+        <v>10539.09</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18">
+        <v>8202.52</v>
+      </c>
+      <c r="C18">
+        <v>2363.38</v>
+      </c>
+      <c r="D18">
+        <v>10565.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B19">
+        <v>8202.52</v>
+      </c>
+      <c r="C19">
+        <v>2397.61</v>
+      </c>
+      <c r="D19">
+        <v>10600.13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20">
+        <v>7386.9400000000014</v>
+      </c>
+      <c r="C20">
+        <v>3188.97</v>
+      </c>
+      <c r="D20">
+        <v>10575.91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21">
+        <v>6767.2400000000016</v>
+      </c>
+      <c r="C21">
+        <v>3845.63</v>
+      </c>
+      <c r="D21">
+        <v>10612.87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22">
+        <v>7733.7200000000012</v>
+      </c>
+      <c r="C22">
+        <v>2890.52</v>
+      </c>
+      <c r="D22">
+        <v>10624.24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23">
+        <v>8370.18</v>
+      </c>
+      <c r="C23">
+        <v>2242.15</v>
+      </c>
+      <c r="D23">
+        <v>10612.33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B24">
+        <v>8370.18</v>
+      </c>
+      <c r="C24">
+        <v>2251.8000000000002</v>
+      </c>
+      <c r="D24">
+        <v>10621.98</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25">
+        <v>8370.18</v>
+      </c>
+      <c r="C25">
+        <v>2241.5100000000002</v>
+      </c>
+      <c r="D25">
+        <v>10611.69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26">
+        <v>8370.18</v>
+      </c>
+      <c r="C26">
+        <v>2238.84</v>
+      </c>
+      <c r="D26">
+        <v>10609.02</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27">
+        <v>5922.63</v>
+      </c>
+      <c r="C27">
+        <v>4568.08</v>
+      </c>
+      <c r="D27">
+        <v>10490.71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28">
+        <v>5922.63</v>
+      </c>
+      <c r="C28">
+        <v>4641.95</v>
+      </c>
+      <c r="D28">
+        <v>10564.58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29">
+        <v>5922.63</v>
+      </c>
+      <c r="C29">
+        <v>4652.21</v>
+      </c>
+      <c r="D29">
+        <v>10574.84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30">
+        <v>5922.63</v>
+      </c>
+      <c r="C30">
+        <v>4734.7</v>
+      </c>
+      <c r="D30">
+        <v>10657.33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B31">
+        <v>4784.01</v>
+      </c>
+      <c r="C31">
+        <v>5821.73</v>
+      </c>
+      <c r="D31">
+        <v>10605.74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32">
+        <v>3877.9700000000012</v>
+      </c>
+      <c r="C32">
+        <v>6631.96</v>
+      </c>
+      <c r="D32">
+        <v>10509.93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33">
+        <v>3877.9700000000012</v>
+      </c>
+      <c r="C33">
+        <v>6702.56</v>
+      </c>
+      <c r="D33">
+        <v>10580.53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34">
+        <v>3877.9700000000012</v>
+      </c>
+      <c r="C34">
+        <v>6685.8899999999994</v>
+      </c>
+      <c r="D34">
+        <v>10563.86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35">
+        <v>3877.9700000000012</v>
+      </c>
+      <c r="C35">
+        <v>6703.36</v>
+      </c>
+      <c r="D35">
+        <v>10581.33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B36">
+        <v>3877.9700000000012</v>
+      </c>
+      <c r="C36">
+        <v>6703.36</v>
+      </c>
+      <c r="D36">
+        <v>10581.33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B37">
+        <v>3877.9700000000012</v>
+      </c>
+      <c r="C37">
+        <v>6780.16</v>
+      </c>
+      <c r="D37">
+        <v>10658.13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38">
+        <v>3877.9700000000012</v>
+      </c>
+      <c r="C38">
+        <v>6719.39</v>
+      </c>
+      <c r="D38">
+        <v>10597.36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39">
+        <v>3877.9700000000012</v>
+      </c>
+      <c r="C39">
+        <v>6710.83</v>
+      </c>
+      <c r="D39">
+        <v>10588.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B40">
+        <v>5740.5700000000024</v>
+      </c>
+      <c r="C40">
+        <v>4792.0300000000007</v>
+      </c>
+      <c r="D40">
+        <v>10532.6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B41">
+        <v>5740.5700000000024</v>
+      </c>
+      <c r="C41">
+        <v>4885.3600000000006</v>
+      </c>
+      <c r="D41">
+        <v>10625.93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>